<commit_message>
general data review, additional paths
</commit_message>
<xml_diff>
--- a/data/raw/ttc/docs/ttc-subway-delay-readme.xlsx
+++ b/data/raw/ttc/docs/ttc-subway-delay-readme.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\clk\CIMS\CIP\Open Data\Open Data Datasets\Recent Datasets\TTC - Subway Delays\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\OneDrive\PET PROJECTS\TTC Delay Analysis\data\raw\ttc\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_6258E70876776701C84EA056BA135EC84F1FD3A3" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{0EA66CED-65B5-4B66-9012-7A283AC637E3}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10455" windowHeight="7575"/>
+    <workbookView xWindow="19090" yWindow="2300" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta Data" sheetId="1" r:id="rId1"/>
@@ -113,7 +114,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -132,12 +133,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -152,12 +159,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -194,12 +202,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:C11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Field Name"/>
-    <tableColumn id="2" name="Description"/>
-    <tableColumn id="3" name="Example"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Field Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Example"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -467,11 +475,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -494,7 +502,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -505,7 +513,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -516,7 +524,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -527,7 +535,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -538,7 +546,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -549,7 +557,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -560,7 +568,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -571,7 +579,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -582,7 +590,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">

</xml_diff>